<commit_message>
Added new fields to the crfs database
</commit_message>
<xml_diff>
--- a/Excel/survey.xlsx
+++ b/Excel/survey.xlsx
@@ -8,16 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoffOffline\GiSTConfigX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E48DB-7978-4880-A545-F160C6373F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB2C5B4-E001-4D0F-8AA7-21B50D47B922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="survey_dd" sheetId="2" r:id="rId1"/>
-    <sheet name="crfs" sheetId="3" r:id="rId2"/>
+    <sheet name="enrollment_dd" sheetId="2" r:id="rId1"/>
+    <sheet name="followup_dd" sheetId="4" r:id="rId2"/>
+    <sheet name="swf_dd" sheetId="5" r:id="rId3"/>
+    <sheet name="crfs" sheetId="3" r:id="rId4"/>
+    <sheet name="README" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey_dd!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">enrollment_dd!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">followup_dd!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">swf_dd!$A$1:$N$11</definedName>
     <definedName name="uganda_villages">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="124">
   <si>
     <t>FieldName</t>
   </si>
@@ -169,15 +174,6 @@
   </si>
   <si>
     <t>checkbox</t>
-  </si>
-  <si>
-    <t>What medication(s) have you taken?</t>
-  </si>
-  <si>
-    <t>1:Oral PrEP
-2:Injectable PrEP (CAB-LA)
-3:PrEP vaginal ring
-4:PEP</t>
   </si>
   <si>
     <t>Participants Sex</t>
@@ -227,35 +223,522 @@
     <t>Please enter the tablet/phone number of the tablet you are using</t>
   </si>
   <si>
-    <t>Please re- enter the tablet/phone number of the tablet you are using</t>
-  </si>
-  <si>
     <t>postskip: if village &lt;&gt; 4, skip to info1</t>
   </si>
   <si>
-    <t>prep_pep_type</t>
-  </si>
-  <si>
-    <t>table</t>
-  </si>
-  <si>
     <t>primarykey</t>
   </si>
   <si>
     <t>displayname</t>
   </si>
   <si>
-    <t>survey</t>
-  </si>
-  <si>
-    <t>Test Survey</t>
+    <t xml:space="preserve">preskip: if pregnant &lt;&gt; 1, skip to village
+</t>
+  </si>
+  <si>
+    <t>followup</t>
+  </si>
+  <si>
+    <t>subjid,vdate</t>
+  </si>
+  <si>
+    <t>Followup Survey</t>
+  </si>
+  <si>
+    <t>vdate</t>
+  </si>
+  <si>
+    <t>Date of visit</t>
+  </si>
+  <si>
+    <t>visittype</t>
+  </si>
+  <si>
+    <t>Visit Type</t>
+  </si>
+  <si>
+    <t>1:12 week
+2:24 week
+3:48 week</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>Comments (optional)</t>
+  </si>
+  <si>
+    <t>Which devices do you use regularly? (Select all that apply)</t>
+  </si>
+  <si>
+    <t>device_use</t>
+  </si>
+  <si>
+    <t>device_use_other</t>
+  </si>
+  <si>
+    <t>Specify other device(s)</t>
+  </si>
+  <si>
+    <t>studyarm</t>
+  </si>
+  <si>
+    <t>Study Arm</t>
+  </si>
+  <si>
+    <t>1:Intervention
+0:Control</t>
+  </si>
+  <si>
+    <t>1:Smartphone
+2:Laptop/desktop computer
+3:Tablet
+4:Smart watch or fitness tracker
+5:Gaming console
+99:Other (specify)</t>
+  </si>
+  <si>
+    <t>preskip: if device_use 'does not contain' 99, skip to comments</t>
+  </si>
+  <si>
+    <t>SEARCH SAPPHIRE ID</t>
+  </si>
+  <si>
+    <t>withdrawreason</t>
+  </si>
+  <si>
+    <t>Reason for subject withdrawal</t>
+  </si>
+  <si>
+    <t>1:Participant determined to be ineligible (select reason)
+2:Withdrawal of informed consent
+3:Study participant death
+4:Other reason for withdrawal
+5:Participant moved from the study community</t>
+  </si>
+  <si>
+    <t>postskip: if withdrawreason &lt;&gt; 4, skip to ineligible</t>
+  </si>
+  <si>
+    <t>orwithdraw</t>
+  </si>
+  <si>
+    <t>Specify other reason for withdrawal</t>
+  </si>
+  <si>
+    <t>postskip: if withdrawreason = 4, skip to withdrawdate</t>
+  </si>
+  <si>
+    <t>ineligible</t>
+  </si>
+  <si>
+    <t>Whay was the participant determined to be ineligible</t>
+  </si>
+  <si>
+    <t>1:Negative HIV test
+2:Other reason for ineligibility (specify)</t>
+  </si>
+  <si>
+    <t>preskip: if withdrawreason &lt;&gt; 1, skip to withdrawdate
+postskip: if ineligible = 1, skip to withdrawdate</t>
+  </si>
+  <si>
+    <t>orineligible</t>
+  </si>
+  <si>
+    <t>Specify: Other reason for ineligibility</t>
+  </si>
+  <si>
+    <t>withdrawdate</t>
+  </si>
+  <si>
+    <t>Withdrawal date
+(if due to death, record death date)</t>
+  </si>
+  <si>
+    <t>preskip: if withdrawreason = 5, skip to movedate_year
+postskip: if withdrawreason &lt;&gt; 5, skip to comments</t>
+  </si>
+  <si>
+    <t>movedate_year</t>
+  </si>
+  <si>
+    <t>MOVE DATE (year)</t>
+  </si>
+  <si>
+    <t>2021:2021
+2022:2022
+2023:2023</t>
+  </si>
+  <si>
+    <t>movedate_month</t>
+  </si>
+  <si>
+    <t>MOVE DATE (month)</t>
+  </si>
+  <si>
+    <t>1:January
+2:February
+3:March
+4:April
+5:May
+6:June
+7:July
+8:August
+9:September
+10:October
+11:November
+12:December</t>
+  </si>
+  <si>
+    <t>movedate_day</t>
+  </si>
+  <si>
+    <t>MOVE DATE (day)</t>
+  </si>
+  <si>
+    <t>1:1
+2:2
+3:3
+4:4
+5:5
+6:6
+7:7
+8:8
+9:9
+10:10
+11:11
+12:12
+13:13
+14:14
+15:15
+16:16
+17:17
+18:18
+19:19
+20:20
+21:21
+22:22
+23:23
+24:24
+25:25
+26:26
+27:27
+28:28
+29:29
+30:30
+31:31</t>
+  </si>
+  <si>
+    <t>fixed: if movedate_month = 2 'and' movedate_day = 29, error_message February does not have 29 days!
+fixed: if movedate_month = 2 'and' movedate_day = 30, error_message February does not have 30 days!
+fixed: if movedate_month = 2 'and' movedate_day = 31, error_message February does not have 31 days!
+fixed: if movedate_month = 4 'and' movedate_day = 31, error_message April only has 30 days!
+fixed: if movedate_month = 6 'and' movedate_day = 31, error_message June only has 30 days!
+fixed: if movedate_month = 9 'and' movedate_day = 31, error_message September only has 30 days!
+fixed: if movedate_month = 11 'and' movedate_day = 31, error_message November only has 30 days!</t>
+  </si>
+  <si>
+    <t>swf</t>
+  </si>
+  <si>
+    <t>Subject Withdrawal Form</t>
+  </si>
+  <si>
+    <t>enrollment</t>
+  </si>
+  <si>
+    <t>Enrollment Form</t>
+  </si>
+  <si>
+    <t>tablename</t>
+  </si>
+  <si>
+    <t>isbase</t>
+  </si>
+  <si>
+    <t>linkingfield</t>
+  </si>
+  <si>
+    <t>parenttable</t>
+  </si>
+  <si>
+    <t>incrementfield</t>
+  </si>
+  <si>
+    <t>requireslink</t>
+  </si>
+  <si>
+    <t>idconfig</t>
+  </si>
+  <si>
+    <t>{"prefix": "GX", "fields": [{"name": "tabletnum", "length": 2}], "incrementLength": 3}</t>
+  </si>
+  <si>
+    <t>idconfig JSON example:
+{
+  "prefix": "SP",
+  "fields": [
+    {"name": "country", "length": 1},
+    {"name": "parish", "length": 2},
+    {"name": "village", "length": 2}
+  ],
+  "incrementLength": 3
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examples of Generated IDs:
+If a user enters:
+   • country = 5
+   • parish = 3
+   • village = 12
+The system would generate:
+   • SP5031201 (first subject)
+   • SP5031202 (second subject)
+   • SP5031203 (third subject)
+Breakdown:
+   • SP = prefix
+   • 5 = country (padded to length 1, so "5" stays "5")
+   • 03 = parish (padded to length 2, so "3" becomes "03")
+   • 12 = village (padded to length 2, so "12" stays "12")
+   • 001, 002, 003 = incremental number (padded to length 3)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another Example:
+If a user enters:
+   • country = 2
+   • parish = 7
+   • village = 5
+Generated IDs:
+   • SP2070501
+   • SP2070502
+   • SP2070503
+Breakdown:
+   • SP = prefix
+   • 2 = country (length 1)
+   • 07 = parish (3 → 03, length 2)
+   • 05 = village (5 → 05, length 2)
+   • 001, 002, 003 = increment
+</t>
+  </si>
+  <si>
+    <t>Explanation of Fields in crfs table</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tablename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: the table name in the database (same as worksheet name ending in _dd)
+   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>primarykey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: comma separated list of fields comprising the primary key
+   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>displayname</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Name of CRF to be displayed when conducting the survey
+   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>isbase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 1 if this is the enrollment/base questionnaire, 0 otherwise
+   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>linkingfield</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The field name that links child records to parent (e.g., 'subjid')
+   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parenttable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The parent table to get linking IDs from (NULL for base forms)
+   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incrementfield</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Field to auto-increment (e.g., 'linenum' for household members) - NULL if not needed
+   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>requireslink</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 1 means user must select a parent ID before starting the questionnaire
+   • </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idconfig</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: JSON configuration for generating unique IDs (only for base forms)
+      o prefix: Static prefix (e.g., "GX")
+      o fields: Array of field names and their padded lengths
+      o incrementLength: Length of the incremental number (3 = 001, 002, etc.)</t>
+    </r>
+  </si>
+  <si>
+    <t>Please re-enter the tablet/phone number of the tablet you are using</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,12 +822,18 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,14 +846,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor theme="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -387,21 +870,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -412,7 +880,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -472,17 +940,57 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +1001,27 @@
     <cellStyle name="Normal 3 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -795,11 +1323,554 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD136"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="5.44140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="55.77734375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12">
+        <v>75</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12">
+        <v>75</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="M7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="18"/>
+    </row>
+    <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N9" s="18"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="20">
+        <v>80</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+    </row>
+    <row r="11" spans="1:14" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="20">
+        <v>80</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" s="18"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="20">
+        <v>80</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2 A4">
+    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:A18">
+    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6134BD1-16F5-4067-922E-C6FBEE76C233}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,13 +1965,13 @@
         <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" s="5">
         <v>10</v>
@@ -915,29 +1986,23 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="11">
-        <v>2</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="12">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12">
-        <v>75</v>
-      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -945,231 +2010,563 @@
       <c r="M4" s="11"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="11" t="s">
+    <row r="5" spans="1:14" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="C7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="20">
+        <v>80</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:A11">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE88F8AD-55EA-4526-AC38-F064E6C4CDEE}">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="87.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.44140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.77734375" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12">
+      <c r="D1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+    </row>
+    <row r="3" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="22">
+        <v>10</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" s="31"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="21">
+        <v>80</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="N6" s="33"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="21">
+        <v>80</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="F9" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="12">
-        <v>75</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="13"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+    </row>
+    <row r="10" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-    </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="D10" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12" t="b">
+      <c r="D11" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="K7" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="13"/>
-    </row>
-    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-    </row>
-    <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="N9" s="18"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="18" t="s">
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+    </row>
+    <row r="12" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="20">
-        <v>80</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-    </row>
-    <row r="11" spans="1:14" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="18" t="s">
-        <v>43</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E12" s="20">
+        <v>80</v>
+      </c>
+      <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="18" t="b">
-        <v>1</v>
-      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>33</v>
       </c>
@@ -1193,7 +2590,7 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
@@ -1217,7 +2614,7 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
@@ -1241,7 +2638,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>24</v>
       </c>
@@ -1266,55 +2663,206 @@
       <c r="N16" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="1" priority="13"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A13:A16">
-    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E662490A-AAB8-49D7-934A-35EC2F1A68FF}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="69.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>64</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>65</v>
+      <c r="C2" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="24">
+        <v>1</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24">
+        <v>0</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="24">
+        <v>0</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24">
+        <v>1</v>
+      </c>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24">
+        <v>1</v>
+      </c>
+      <c r="I4" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD25F6D-9618-4799-8836-143EC38C60A4}">
+  <dimension ref="B2:U5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="129.6640625" customWidth="1"/>
+    <col min="7" max="7" width="71.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B2" s="39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q3" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="R3" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="S3" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="T3" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="U3" s="37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="G4" s="27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="G5" s="38" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added comples logic checks
</commit_message>
<xml_diff>
--- a/Excel/survey.xlsx
+++ b/Excel/survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoffOffline\GiSTConfigX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB2C5B4-E001-4D0F-8AA7-21B50D47B922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080CDC85-17A3-4FC6-94F9-DBDFF64D915C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enrollment_dd" sheetId="2" r:id="rId1"/>
@@ -170,9 +170,6 @@
     <t>tabletnum2</t>
   </si>
   <si>
-    <t>dynamic: if tabletnum2 &lt;&gt; tabletnum, error_message This does not match your previous entry!</t>
-  </si>
-  <si>
     <t>checkbox</t>
   </si>
   <si>
@@ -428,15 +425,6 @@
 29:29
 30:30
 31:31</t>
-  </si>
-  <si>
-    <t>fixed: if movedate_month = 2 'and' movedate_day = 29, error_message February does not have 29 days!
-fixed: if movedate_month = 2 'and' movedate_day = 30, error_message February does not have 30 days!
-fixed: if movedate_month = 2 'and' movedate_day = 31, error_message February does not have 31 days!
-fixed: if movedate_month = 4 'and' movedate_day = 31, error_message April only has 30 days!
-fixed: if movedate_month = 6 'and' movedate_day = 31, error_message June only has 30 days!
-fixed: if movedate_month = 9 'and' movedate_day = 31, error_message September only has 30 days!
-fixed: if movedate_month = 11 'and' movedate_day = 31, error_message November only has 30 days!</t>
   </si>
   <si>
     <t>swf</t>
@@ -732,6 +720,12 @@
   </si>
   <si>
     <t>Please re-enter the tablet/phone number of the tablet you are using</t>
+  </si>
+  <si>
+    <t>(movedate_month = '2' and movedate_day = '29') or (movedate_month = '2' and movedate_day = '30') or (movedate_month = '2' and movedate_day = '31') or (movedate_month = '4' and movedate_day = '31') or (movedate_month = '6' and movedate_day = '31') or (movedate_month = '9' and movedate_day = '31') or (movedate_month = '11' and movedate_day = '31'); 'Invalid day for the selected month.'</t>
+  </si>
+  <si>
+    <t>tabletnum2 != tabletnum; 'This does not match your previous entry!'</t>
   </si>
 </sst>
 </file>
@@ -1325,9 +1319,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1428,7 +1422,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="11">
         <v>2</v>
@@ -1458,7 +1452,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="5">
         <v>10</v>
@@ -1484,7 +1478,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" s="11">
         <v>2</v>
@@ -1497,7 +1491,7 @@
         <v>75</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
@@ -1516,7 +1510,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -1533,7 +1527,7 @@
     </row>
     <row r="7" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>26</v>
@@ -1542,30 +1536,26 @@
         <v>19</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>20</v>
@@ -1574,20 +1564,22 @@
         <v>20</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18" t="b">
+      <c r="J8" s="12" t="b">
         <v>1</v>
       </c>
+      <c r="K8" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="18"/>
       <c r="M8" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N8" s="18"/>
     </row>
@@ -1596,17 +1588,17 @@
         <v>27</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
@@ -1615,13 +1607,13 @@
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N9" s="18"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>21</v>
@@ -1630,7 +1622,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="20">
         <v>80</v>
@@ -1671,37 +1663,33 @@
     </row>
     <row r="12" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="K12" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="18" t="b">
-        <v>1</v>
-      </c>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>21</v>
@@ -1710,7 +1698,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="20">
         <v>80</v>
@@ -1723,13 +1711,13 @@
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N13" s="18"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>21</v>
@@ -1738,7 +1726,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="20">
         <v>80</v>
@@ -1870,24 +1858,24 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="79.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.6640625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="5.44140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="43" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="8.88671875" style="6"/>
   </cols>
@@ -1971,7 +1959,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="5">
         <v>10</v>
@@ -1988,7 +1976,7 @@
     </row>
     <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>20</v>
@@ -1997,7 +1985,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -2012,7 +2000,7 @@
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -2021,11 +2009,11 @@
         <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -2038,7 +2026,7 @@
     </row>
     <row r="6" spans="1:14" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>26</v>
@@ -2047,11 +2035,11 @@
         <v>19</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -2064,7 +2052,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>21</v>
@@ -2073,7 +2061,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="20">
         <v>80</v>
@@ -2200,9 +2188,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE88F8AD-55EA-4526-AC38-F064E6C4CDEE}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,10 +2203,10 @@
     <col min="6" max="6" width="46.6640625" style="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="87.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="86.88671875" style="27" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.88671875" style="27" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.6640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.44140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5546875" style="27" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="45.77734375" style="27" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.109375" style="27" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.109375" style="27"/>
@@ -2303,7 +2291,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="22">
         <v>10</v>
@@ -2320,7 +2308,7 @@
     </row>
     <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>26</v>
@@ -2329,11 +2317,11 @@
         <v>19</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
@@ -2342,13 +2330,13 @@
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
       <c r="M4" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N4" s="31"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>21</v>
@@ -2357,7 +2345,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="21">
         <v>80</v>
@@ -2370,13 +2358,13 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="M5" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>26</v>
@@ -2385,11 +2373,11 @@
         <v>19</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
@@ -2398,13 +2386,13 @@
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>21</v>
@@ -2413,7 +2401,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" s="21">
         <v>80</v>
@@ -2430,7 +2418,7 @@
     </row>
     <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>20</v>
@@ -2439,7 +2427,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="29"/>
@@ -2450,13 +2438,13 @@
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>26</v>
@@ -2465,18 +2453,16 @@
         <v>19</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
-      <c r="J9" s="21" t="b">
-        <v>1</v>
-      </c>
+      <c r="J9" s="21"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
@@ -2484,7 +2470,7 @@
     </row>
     <row r="10" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>26</v>
@@ -2493,18 +2479,16 @@
         <v>19</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
-      <c r="J10" s="21" t="b">
-        <v>1</v>
-      </c>
+      <c r="J10" s="21"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
@@ -2512,29 +2496,27 @@
     </row>
     <row r="11" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="J11" s="21" t="b">
-        <v>1</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="J11" s="21"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
@@ -2542,7 +2524,7 @@
     </row>
     <row r="12" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>21</v>
@@ -2551,7 +2533,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="20">
         <v>80</v>
@@ -2693,42 +2675,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>114</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" s="37" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D2" s="24">
         <v>1</v>
@@ -2742,18 +2724,18 @@
         <v>0</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>62</v>
       </c>
       <c r="D3" s="24">
         <v>0</v>
@@ -2762,7 +2744,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G3" s="24"/>
       <c r="H3" s="24">
@@ -2772,13 +2754,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D4" s="24">
         <v>0</v>
@@ -2787,7 +2769,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G4" s="24"/>
       <c r="H4" s="24">
@@ -2817,52 +2799,52 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" s="39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M3" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q3" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="N3" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" s="37" t="s">
+      <c r="R3" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="S3" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="R3" s="37" t="s">
+      <c r="T3" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="S3" s="37" t="s">
+      <c r="U3" s="37" t="s">
         <v>114</v>
-      </c>
-      <c r="T3" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="U3" s="37" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="2:21" ht="259.2" x14ac:dyDescent="0.3">
       <c r="G4" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="2:21" ht="244.8" x14ac:dyDescent="0.3">
       <c r="G5" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to add date ranges for 'date' questions
</commit_message>
<xml_diff>
--- a/Excel/survey.xlsx
+++ b/Excel/survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoffOffline\GiSTConfigX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080CDC85-17A3-4FC6-94F9-DBDFF64D915C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B761506-A817-483C-867A-7CBE9F9F5F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="128">
   <si>
     <t>FieldName</t>
   </si>
@@ -727,6 +727,18 @@
   <si>
     <t>tabletnum2 != tabletnum; 'This does not match your previous entry!'</t>
   </si>
+  <si>
+    <t>+0d</t>
+  </si>
+  <si>
+    <t>-9m</t>
+  </si>
+  <si>
+    <t>-2m</t>
+  </si>
+  <si>
+    <t>-1y</t>
+  </si>
 </sst>
 </file>
 
@@ -874,7 +886,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -985,6 +997,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1321,7 +1339,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1568,8 +1586,12 @@
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
+      <c r="G8" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>124</v>
+      </c>
       <c r="I8" s="18"/>
       <c r="J8" s="12" t="b">
         <v>1</v>
@@ -1681,8 +1703,12 @@
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="J12" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
@@ -1858,7 +1884,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,8 +2015,12 @@
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="G4" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>124</v>
+      </c>
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -2190,7 +2220,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2431,10 +2461,16 @@
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="29"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="G8" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>124</v>
+      </c>
       <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="J8" s="21" t="b">
+        <v>1</v>
+      </c>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21" t="s">
@@ -2494,7 +2530,7 @@
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="184.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
Added functionality to have a 'unique' logic check
</commit_message>
<xml_diff>
--- a/Excel/survey.xlsx
+++ b/Excel/survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoffOffline\GiSTConfigX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B761506-A817-483C-867A-7CBE9F9F5F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C999EF0D-29FF-44B7-87E0-5889615CE8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enrollment_dd" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
   <si>
     <t>FieldName</t>
   </si>
@@ -738,6 +738,15 @@
   </si>
   <si>
     <t>-1y</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>Enter the barcode</t>
+  </si>
+  <si>
+    <t>unique; 'barcode will create duplicates'</t>
   </si>
 </sst>
 </file>
@@ -1337,9 +1346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,11 +1889,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6134BD1-16F5-4067-922E-C6FBEE76C233}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1897,7 +1906,7 @@
     <col min="6" max="6" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.21875" style="6" customWidth="1"/>
     <col min="10" max="10" width="9.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.6640625" style="6" customWidth="1"/>
     <col min="12" max="12" width="3.5546875" style="6" bestFit="1" customWidth="1"/>
@@ -2080,59 +2089,63 @@
       <c r="M6" s="22"/>
       <c r="N6" s="22"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="22">
+        <v>4</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D8" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E8" s="20">
         <v>80</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>15</v>
@@ -2141,7 +2154,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -2156,16 +2169,16 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -2179,34 +2192,58 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>24</v>
+      <c r="A11" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A11">
+  <conditionalFormatting sqref="A9:A12">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added config file for generation of survey_manifest.gistx config file
</commit_message>
<xml_diff>
--- a/Excel/survey.xlsx
+++ b/Excel/survey.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoffOffline\GiSTConfigX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C999EF0D-29FF-44B7-87E0-5889615CE8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF008BA-B87C-4754-B43A-B47CC98843E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enrollment_dd" sheetId="2" r:id="rId1"/>
     <sheet name="followup_dd" sheetId="4" r:id="rId2"/>
     <sheet name="swf_dd" sheetId="5" r:id="rId3"/>
-    <sheet name="crfs" sheetId="3" r:id="rId4"/>
-    <sheet name="README" sheetId="6" r:id="rId5"/>
+    <sheet name="crfss" sheetId="3" r:id="rId4"/>
+    <sheet name="household_ddd" sheetId="7" r:id="rId5"/>
+    <sheet name="hh_members_ddd" sheetId="8" r:id="rId6"/>
+    <sheet name="crfs" sheetId="9" r:id="rId7"/>
+    <sheet name="README" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">enrollment_dd!$A$1:$I$1</definedName>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="173">
   <si>
     <t>FieldName</t>
   </si>
@@ -115,9 +118,6 @@
   </si>
   <si>
     <t>swver</t>
-  </si>
-  <si>
-    <t>Software Version</t>
   </si>
   <si>
     <t>stoptime</t>
@@ -748,12 +748,151 @@
   <si>
     <t>unique; 'barcode will create duplicates'</t>
   </si>
+  <si>
+    <t>barcode2</t>
+  </si>
+  <si>
+    <t>Re-enter the barcode</t>
+  </si>
+  <si>
+    <t>barcode2 != barcode; 'The barcodes do not match'</t>
+  </si>
+  <si>
+    <t>Date/time of start of visit</t>
+  </si>
+  <si>
+    <t>hhid</t>
+  </si>
+  <si>
+    <t>headofhouseholdname</t>
+  </si>
+  <si>
+    <t>What is the name of the head of the household</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Any additional comments (optional)</t>
+  </si>
+  <si>
+    <t>Globally Unique Identifier (GUID</t>
+  </si>
+  <si>
+    <t>Survey End Time</t>
+  </si>
+  <si>
+    <t>Date/Time stamp when record was last modified</t>
+  </si>
+  <si>
+    <t>linenum</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Participants name</t>
+  </si>
+  <si>
+    <t>Participants sex</t>
+  </si>
+  <si>
+    <t>1:Female
+2:Male</t>
+  </si>
+  <si>
+    <t>census_age</t>
+  </si>
+  <si>
+    <t>Uganda: Age: Register instructions: Record age in complete year and months (mth) for children less than one year and days for children less than one month.
+Kenya: No instructions on register</t>
+  </si>
+  <si>
+    <t>household_relation</t>
+  </si>
+  <si>
+    <t>Relationship to head of household</t>
+  </si>
+  <si>
+    <t>1:Head of household
+2:Spouse
+3:Son/daughter
+4:Other relative
+5:Other (specify)</t>
+  </si>
+  <si>
+    <t>Kenya: relationship to head of household, with the following response options: 1:head of household; 2:spouse; 3:Child(B) and 4: Child). I don't know the difference between the 3 and 4 code: I will ask the Kenya team. I also don't see a response option for other adults in the home.</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>1:Mbarara
+2:Kampala
+3:Jinja
+4:Mbale</t>
+  </si>
+  <si>
+    <t>How many people stay in this household?</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>Household Survey</t>
+  </si>
+  <si>
+    <t>hh_members</t>
+  </si>
+  <si>
+    <t>hhid,linenum</t>
+  </si>
+  <si>
+    <t>Household Member Survey</t>
+  </si>
+  <si>
+    <t>{"prefix": "GL", "fields": [{"name": "community", "length": 2}], "incrementLength": 3}</t>
+  </si>
+  <si>
+    <t>participantsname</t>
+  </si>
+  <si>
+    <t>How old is [[participantsname]] in completed years?
+(Enter 0 if age &amp;lt; 1 year)</t>
+  </si>
+  <si>
+    <t>repeat_count_field</t>
+  </si>
+  <si>
+    <t>auto_start_repeat</t>
+  </si>
+  <si>
+    <t>repeat_enforce_count</t>
+  </si>
+  <si>
+    <t>display_order</t>
+  </si>
+  <si>
+    <t>display_fields</t>
+  </si>
+  <si>
+    <t>num_people</t>
+  </si>
+  <si>
+    <t>survey_id</t>
+  </si>
+  <si>
+    <t>Survey Version</t>
+  </si>
+  <si>
+    <t>GiSTX Software Version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -847,8 +986,39 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4285F4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -861,8 +1031,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -885,8 +1067,104 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -894,8 +1172,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1012,8 +1291,48 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="7" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -1021,8 +1340,44 @@
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal 3 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 5" xfId="7" xr:uid="{0F15704D-2A5C-44A8-8963-B0F37299923F}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1344,11 +1699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1440,16 +1795,16 @@
     </row>
     <row r="3" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="11">
         <v>2</v>
@@ -1479,7 +1834,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="5">
         <v>10</v>
@@ -1496,16 +1851,16 @@
     </row>
     <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="11">
         <v>2</v>
@@ -1518,7 +1873,7 @@
         <v>75</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
@@ -1528,20 +1883,20 @@
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -1554,20 +1909,20 @@
     </row>
     <row r="7" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1576,13 +1931,13 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>20</v>
@@ -1591,15 +1946,15 @@
         <v>20</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="12" t="b">
@@ -1610,26 +1965,26 @@
       </c>
       <c r="L8" s="18"/>
       <c r="M8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N8" s="18"/>
     </row>
     <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
@@ -1638,22 +1993,22 @@
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N9" s="18"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>53</v>
       </c>
       <c r="E10" s="20">
         <v>80</v>
@@ -1670,16 +2025,16 @@
     </row>
     <row r="11" spans="1:14" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -1694,20 +2049,20 @@
     </row>
     <row r="12" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
@@ -1724,16 +2079,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>71</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>72</v>
       </c>
       <c r="E13" s="20">
         <v>80</v>
@@ -1746,22 +2101,22 @@
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N13" s="18"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="E14" s="20">
         <v>80</v>
@@ -1778,7 +2133,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>15</v>
@@ -1787,7 +2142,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1811,7 +2166,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>23</v>
+        <v>172</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
@@ -1826,16 +2181,16 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>34</v>
+        <v>170</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>35</v>
+        <v>171</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -1849,38 +2204,62 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>24</v>
+      <c r="A18" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2 A4">
-    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:A18">
-    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+  <conditionalFormatting sqref="A15:A19">
+    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1889,11 +2268,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6134BD1-16F5-4067-922E-C6FBEE76C233}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1994,7 +2373,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="5">
         <v>10</v>
@@ -2011,7 +2390,7 @@
     </row>
     <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>20</v>
@@ -2020,15 +2399,15 @@
         <v>20</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
@@ -2039,20 +2418,20 @@
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -2065,20 +2444,20 @@
     </row>
     <row r="6" spans="1:14" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -2091,16 +2470,16 @@
     </row>
     <row r="7" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>128</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>129</v>
       </c>
       <c r="E7" s="22">
         <v>4</v>
@@ -2109,7 +2488,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
@@ -2117,59 +2496,63 @@
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="22">
+        <v>4</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="20">
+      <c r="E9" s="20">
         <v>80</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>15</v>
@@ -2178,7 +2561,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -2193,16 +2576,16 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>35</v>
+        <v>172</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -2216,35 +2599,86 @@
       <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>24</v>
+      <c r="A12" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>16</v>
+      <c r="C12" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>25</v>
+        <v>171</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A12">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="A10 A13:A14">
+    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:A12">
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2253,11 +2687,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE88F8AD-55EA-4526-AC38-F064E6C4CDEE}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2358,7 +2792,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="22">
         <v>10</v>
@@ -2375,20 +2809,20 @@
     </row>
     <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
@@ -2397,22 +2831,22 @@
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
       <c r="M4" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N4" s="31"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="E5" s="21">
         <v>80</v>
@@ -2425,26 +2859,26 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="M5" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
@@ -2453,22 +2887,22 @@
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>90</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>91</v>
       </c>
       <c r="E7" s="21">
         <v>80</v>
@@ -2485,7 +2919,7 @@
     </row>
     <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>20</v>
@@ -2494,15 +2928,15 @@
         <v>20</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="29"/>
       <c r="G8" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H8" s="41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21" t="b">
@@ -2511,26 +2945,26 @@
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
@@ -2543,20 +2977,20 @@
     </row>
     <row r="10" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
@@ -2569,25 +3003,25 @@
     </row>
     <row r="11" spans="1:14" ht="184.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
@@ -2597,16 +3031,16 @@
     </row>
     <row r="12" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="E12" s="20">
         <v>80</v>
@@ -2623,7 +3057,7 @@
     </row>
     <row r="13" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>15</v>
@@ -2632,7 +3066,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -2656,7 +3090,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>23</v>
+        <v>172</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -2671,16 +3105,16 @@
     </row>
     <row r="15" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>34</v>
+        <v>170</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>35</v>
+        <v>171</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -2694,32 +3128,59 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>24</v>
+      <c r="A16" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
+    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A13:A16">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A13 A16:A17">
+    <cfRule type="duplicateValues" dxfId="5" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:A15">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2727,10 +3188,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E662490A-AAB8-49D7-934A-35EC2F1A68FF}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2744,46 +3205,62 @@
     <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" s="24">
         <v>1</v>
@@ -2797,18 +3274,22 @@
         <v>0</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="D3" s="24">
         <v>0</v>
@@ -2817,23 +3298,27 @@
         <v>18</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G3" s="24"/>
       <c r="H3" s="24">
         <v>1</v>
       </c>
       <c r="I3" s="24"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="24">
         <v>0</v>
@@ -2842,13 +3327,17 @@
         <v>18</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="24"/>
       <c r="H4" s="24">
         <v>1</v>
       </c>
       <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2856,11 +3345,968 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61A739D-6D79-4A57-8134-05562094E09D}">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" style="43" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="43" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="43" customWidth="1"/>
+    <col min="4" max="4" width="72.21875" style="43" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="43" customWidth="1"/>
+    <col min="6" max="6" width="34.21875" style="43" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" style="43" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="43" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="43" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="43" customWidth="1"/>
+    <col min="12" max="12" width="5.21875" style="43" customWidth="1"/>
+    <col min="13" max="13" width="4.6640625" style="43" customWidth="1"/>
+    <col min="14" max="14" width="10.21875" style="43" customWidth="1"/>
+    <col min="15" max="16384" width="12.44140625" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="48"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="46"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="47">
+        <v>80</v>
+      </c>
+      <c r="F5" s="47"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="49" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="47">
+        <v>2</v>
+      </c>
+      <c r="F6" s="47"/>
+      <c r="G6" s="49">
+        <v>1</v>
+      </c>
+      <c r="H6" s="49">
+        <v>50</v>
+      </c>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="56"/>
+    </row>
+    <row r="8" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="20">
+        <v>80</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+    </row>
+    <row r="9" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:N7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="3" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9 A12:A13">
+    <cfRule type="duplicateValues" dxfId="2" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:A11">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710188CE-F1CA-4CEF-97E1-11074B317655}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" style="43" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="43" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="43" customWidth="1"/>
+    <col min="4" max="4" width="63" style="43" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="43" customWidth="1"/>
+    <col min="6" max="6" width="42.44140625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="43" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="43" customWidth="1"/>
+    <col min="9" max="9" width="39.6640625" style="43" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="43" customWidth="1"/>
+    <col min="11" max="12" width="6.33203125" style="43" customWidth="1"/>
+    <col min="13" max="13" width="60.21875" style="43" customWidth="1"/>
+    <col min="14" max="14" width="40.77734375" style="43" customWidth="1"/>
+    <col min="15" max="16384" width="12.44140625" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="46"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="47">
+        <v>80</v>
+      </c>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="46"/>
+    </row>
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="46"/>
+    </row>
+    <row r="7" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="47">
+        <v>3</v>
+      </c>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47">
+        <v>0</v>
+      </c>
+      <c r="H7" s="47">
+        <v>110</v>
+      </c>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="48" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="59"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="47">
+        <v>255</v>
+      </c>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="46">
+        <v>36</v>
+      </c>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+    </row>
+    <row r="12" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="47"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="46"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:N9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A12:A13">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA763A67-FC13-4157-8CE1-E1599E3E3270}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="L1" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>169</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD25F6D-9618-4799-8836-143EC38C60A4}">
   <dimension ref="B2:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2872,52 +4318,52 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M3" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="N3" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="O3" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" s="37" t="s">
+      <c r="Q3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="R3" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="37" t="s">
+      <c r="S3" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="37" t="s">
+      <c r="T3" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="T3" s="37" t="s">
+      <c r="U3" s="37" t="s">
         <v>113</v>
-      </c>
-      <c r="U3" s="37" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="2:21" ht="259.2" x14ac:dyDescent="0.3">
       <c r="G4" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="2:21" ht="244.8" x14ac:dyDescent="0.3">
       <c r="G5" s="38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented age calculation types and fixed skip validation bug
- Added support for 'age_from_date' and 'age_at_date' calculation types, including parsing logic in ExcelReader.cs and XML generation in XmlGenerator.cs.
- Fixed a bug in ExcelReader.cs::CheckSkipToFieldNames where skip field validations were incorrectly scoped outside the iteration loop, leading to missed errors for all but the last skip condition. Also improved field name extraction robustness.
</commit_message>
<xml_diff>
--- a/Excel/survey.xlsx
+++ b/Excel/survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoffOffline\GiSTConfigX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF008BA-B87C-4754-B43A-B47CC98843E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD62C04C-B8F6-4E47-BE25-8AB303CFE685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enrollment_dd" sheetId="2" r:id="rId1"/>
@@ -161,10 +161,6 @@
   </si>
   <si>
     <t>info1</t>
-  </si>
-  <si>
-    <t>Please record this tablet number:
-[[tabletnum]]</t>
   </si>
   <si>
     <t>tabletnum2</t>
@@ -886,6 +882,10 @@
   </si>
   <si>
     <t>GiSTX Software Version</t>
+  </si>
+  <si>
+    <t>Please record the Subject ID:
+[[subjid]]</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +1703,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1804,7 +1804,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="11">
         <v>2</v>
@@ -1823,63 +1823,63 @@
       <c r="M3" s="11"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12">
+        <v>75</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="13"/>
+    </row>
+    <row r="5" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="5">
         <v>10</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="11">
-        <v>2</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12">
-        <v>1</v>
-      </c>
-      <c r="H5" s="12">
-        <v>75</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="13"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1892,7 +1892,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -1909,7 +1909,7 @@
     </row>
     <row r="7" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>25</v>
@@ -1918,11 +1918,11 @@
         <v>19</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1931,13 +1931,13 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>20</v>
@@ -1946,15 +1946,15 @@
         <v>20</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="12" t="b">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="L8" s="18"/>
       <c r="M8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N8" s="18"/>
     </row>
@@ -1974,17 +1974,17 @@
         <v>26</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
@@ -1993,22 +1993,22 @@
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N9" s="18"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>52</v>
       </c>
       <c r="E10" s="20">
         <v>80</v>
@@ -2034,7 +2034,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>37</v>
+        <v>172</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -2049,20 +2049,20 @@
     </row>
     <row r="12" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
@@ -2079,16 +2079,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>71</v>
       </c>
       <c r="E13" s="20">
         <v>80</v>
@@ -2101,22 +2101,22 @@
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N13" s="18"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>67</v>
       </c>
       <c r="E14" s="20">
         <v>80</v>
@@ -2166,7 +2166,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>15</v>
@@ -2190,7 +2190,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -2252,7 +2252,7 @@
       <c r="N19" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2 A4">
+  <conditionalFormatting sqref="A2 A5">
     <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
@@ -2270,7 +2270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6134BD1-16F5-4067-922E-C6FBEE76C233}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
@@ -2373,7 +2373,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="5">
         <v>10</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>20</v>
@@ -2399,15 +2399,15 @@
         <v>20</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
@@ -2418,7 +2418,7 @@
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>25</v>
@@ -2427,11 +2427,11 @@
         <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="6" spans="1:14" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>25</v>
@@ -2453,11 +2453,11 @@
         <v>19</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -2470,16 +2470,16 @@
     </row>
     <row r="7" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>127</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>128</v>
       </c>
       <c r="E7" s="22">
         <v>4</v>
@@ -2488,7 +2488,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
@@ -2498,16 +2498,16 @@
     </row>
     <row r="8" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>130</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>131</v>
       </c>
       <c r="E8" s="22">
         <v>4</v>
@@ -2516,7 +2516,7 @@
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
@@ -2526,16 +2526,16 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>67</v>
       </c>
       <c r="E9" s="20">
         <v>80</v>
@@ -2585,7 +2585,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>15</v>
@@ -2609,7 +2609,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -2792,7 +2792,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="22">
         <v>10</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>25</v>
@@ -2818,11 +2818,11 @@
         <v>19</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
@@ -2831,22 +2831,22 @@
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
       <c r="M4" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N4" s="31"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>82</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>83</v>
       </c>
       <c r="E5" s="21">
         <v>80</v>
@@ -2859,13 +2859,13 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="M5" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>25</v>
@@ -2874,11 +2874,11 @@
         <v>19</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
@@ -2887,22 +2887,22 @@
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>90</v>
       </c>
       <c r="E7" s="21">
         <v>80</v>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>20</v>
@@ -2928,15 +2928,15 @@
         <v>20</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="29"/>
       <c r="G8" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" s="41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21" t="b">
@@ -2945,13 +2945,13 @@
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>25</v>
@@ -2960,11 +2960,11 @@
         <v>19</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="10" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>25</v>
@@ -2986,11 +2986,11 @@
         <v>19</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
@@ -3003,25 +3003,25 @@
     </row>
     <row r="11" spans="1:14" ht="184.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
@@ -3031,16 +3031,16 @@
     </row>
     <row r="12" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>67</v>
       </c>
       <c r="E12" s="20">
         <v>80</v>
@@ -3090,7 +3090,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="15" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>15</v>
@@ -3114,7 +3114,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -3190,8 +3190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E662490A-AAB8-49D7-934A-35EC2F1A68FF}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3213,54 +3213,54 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="53" t="s">
+      <c r="E1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="F1" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="G1" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="H1" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="I1" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="53" t="s">
-        <v>113</v>
-      </c>
       <c r="J1" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="L1" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="L1" s="52" t="s">
-        <v>166</v>
-      </c>
       <c r="M1" s="52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="24">
         <v>1</v>
@@ -3274,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
@@ -3283,13 +3283,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>59</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>60</v>
       </c>
       <c r="D3" s="24">
         <v>0</v>
@@ -3298,7 +3298,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3" s="24"/>
       <c r="H3" s="24">
@@ -3312,13 +3312,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="24">
         <v>0</v>
@@ -3327,7 +3327,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="24"/>
       <c r="H4" s="24">
@@ -3441,7 +3441,7 @@
     </row>
     <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>25</v>
@@ -3450,11 +3450,11 @@
         <v>19</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E3" s="47"/>
       <c r="F3" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G3" s="47"/>
       <c r="H3" s="47"/>
@@ -3467,7 +3467,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="47" t="s">
         <v>15</v>
@@ -3489,16 +3489,16 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="49" t="s">
         <v>135</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>136</v>
       </c>
       <c r="E5" s="47">
         <v>80</v>
@@ -3515,7 +3515,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="44" t="s">
         <v>21</v>
@@ -3524,7 +3524,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E6" s="47">
         <v>2</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="55"/>
@@ -3563,16 +3563,16 @@
     </row>
     <row r="8" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>67</v>
       </c>
       <c r="E8" s="20">
         <v>80</v>
@@ -3622,7 +3622,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="11" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>15</v>
@@ -3646,7 +3646,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -3807,7 +3807,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>15</v>
@@ -3844,7 +3844,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" s="47" t="s">
         <v>15</v>
@@ -3866,7 +3866,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="47" t="s">
         <v>21</v>
@@ -3875,7 +3875,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E5" s="47">
         <v>80</v>
@@ -3901,11 +3901,11 @@
         <v>19</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6" s="47"/>
       <c r="F6" s="47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="47"/>
@@ -3918,7 +3918,7 @@
     </row>
     <row r="7" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B7" s="47" t="s">
         <v>21</v>
@@ -3927,7 +3927,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E7" s="47">
         <v>3</v>
@@ -3945,12 +3945,12 @@
       <c r="L7" s="47"/>
       <c r="M7" s="47"/>
       <c r="N7" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" s="47" t="s">
         <v>25</v>
@@ -3959,11 +3959,11 @@
         <v>19</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G8" s="47"/>
       <c r="H8" s="47"/>
@@ -3973,12 +3973,12 @@
       <c r="L8" s="47"/>
       <c r="M8" s="47"/>
       <c r="N8" s="46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="58"/>
       <c r="C9" s="58"/>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="47" t="s">
         <v>21</v>
@@ -4005,7 +4005,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" s="47">
         <v>255</v>
@@ -4033,7 +4033,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="46">
         <v>36</v>
@@ -4059,7 +4059,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -4074,7 +4074,7 @@
     </row>
     <row r="13" spans="1:14" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>15</v>
@@ -4083,7 +4083,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -4107,7 +4107,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="47"/>
       <c r="F14" s="49"/>
@@ -4131,7 +4131,7 @@
         <v>16</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="44"/>
@@ -4184,46 +4184,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="L1" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="52" t="s">
         <v>167</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>165</v>
-      </c>
-      <c r="M1" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="N1" s="52" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -4231,25 +4231,25 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
         <v>156</v>
-      </c>
-      <c r="C2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" t="s">
-        <v>157</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -4263,28 +4263,28 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
         <v>158</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>159</v>
-      </c>
-      <c r="D3" t="s">
-        <v>160</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -4293,7 +4293,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4318,52 +4318,52 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M3" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="N3" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="O3" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="37" t="s">
+      <c r="Q3" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="R3" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="R3" s="37" t="s">
+      <c r="S3" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="S3" s="37" t="s">
+      <c r="T3" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="37" t="s">
+      <c r="U3" s="37" t="s">
         <v>112</v>
-      </c>
-      <c r="U3" s="37" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="2:21" ht="259.2" x14ac:dyDescent="0.3">
       <c r="G4" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:21" ht="244.8" x14ac:dyDescent="0.3">
       <c r="G5" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>